<commit_message>
Repalced all xlsx and csv for newest parts with sheet names matching file names.
git-svn-id: svn+ssh://bbfs-01.calit2.net/grw/Gordon/svn/trunk/Gadgets/Libraries/Parts@21528 2cf53259-273a-af40-bda6-69d31023b8ec
</commit_message>
<xml_diff>
--- a/Digikey/Regulators.xlsx
+++ b/Digikey/Regulators.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="10800" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="10800"/>
   </bookViews>
   <sheets>
-    <sheet name="Reg-SMD" sheetId="2" r:id="rId1"/>
-    <sheet name="Reg-TH" sheetId="3" r:id="rId2"/>
+    <sheet name="Regulators-SMD" sheetId="2" r:id="rId1"/>
+    <sheet name="Regulators-TH" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -1652,7 +1652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="AD37" sqref="AD37"/>
     </sheetView>
   </sheetViews>
@@ -4685,7 +4685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>

</xml_diff>